<commit_message>
Naming Convention changed according to caliper standards
</commit_message>
<xml_diff>
--- a/utils/Documentation/Normalize_program/Consolidated_excel_populate/Performance.xlsx
+++ b/utils/Documentation/Normalize_program/Consolidated_excel_populate/Performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="941" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="941" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,10 +19,11 @@
     <sheet name="network" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">algorithm!$A$2:$M$29</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">algorithm!$A$2:$M$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">algorithm!$A$2:$M$29</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">algorithm!$A$2:$M$26</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">algorithm!$A$2:$M$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">algorithm!$A$2:$M$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">algorithm!$A$2:$M$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">algorithm!$A$2:$M$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">algorithm!$A$2:$M$26</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -211,31 +212,31 @@
     <t>compile</t>
   </si>
   <si>
-    <t>kernel-dev_32</t>
+    <t>Kernel-dev_1</t>
   </si>
   <si>
     <t>Kilo sec</t>
   </si>
   <si>
-    <t>kernel-dev_16</t>
+    <t>Kernel-dev_2</t>
   </si>
   <si>
-    <t>kernel-dev_8</t>
+    <t>Kernel-dev_4</t>
   </si>
   <si>
-    <t>kernel-dev_4</t>
+    <t>Kernel-dev_8</t>
   </si>
   <si>
-    <t>kernel-dev_72</t>
+    <t>Kernel-dev_16</t>
   </si>
   <si>
-    <t>kernel-dev_64</t>
+    <t>Kernel-dev_32</t>
   </si>
   <si>
-    <t>kernel-dev_1</t>
+    <t>Kernel-dev_64</t>
   </si>
   <si>
-    <t>kernel-dev_2</t>
+    <t>Kernel-dev_72</t>
   </si>
   <si>
     <t>ebizzy</t>
@@ -244,55 +245,55 @@
     <t>ebizzy_no_mmap_time</t>
   </si>
   <si>
-    <t>sys_4</t>
+    <t>sys_1</t>
   </si>
   <si>
     <t>sys_2</t>
   </si>
   <si>
-    <t>sys_1</t>
+    <t>sys_4</t>
+  </si>
+  <si>
+    <t>sys_8</t>
+  </si>
+  <si>
+    <t>sys_16</t>
+  </si>
+  <si>
+    <t>sys_32</t>
+  </si>
+  <si>
+    <t>sys_64</t>
   </si>
   <si>
     <t>sys_80</t>
   </si>
   <si>
-    <t>sys_8</t>
+    <t>ebizzy_no_mmap_records</t>
   </si>
   <si>
-    <t>sys_32</t>
+    <t>records_1</t>
   </si>
   <si>
-    <t>sys_16</t>
+    <t>records_2</t>
   </si>
   <si>
-    <t>sys_64</t>
-  </si>
-  <si>
-    <t>ebizzy_no_mmap_records</t>
+    <t>records_4</t>
   </si>
   <si>
     <t>records_8</t>
   </si>
   <si>
-    <t>records_4</t>
-  </si>
-  <si>
-    <t>records_2</t>
-  </si>
-  <si>
     <t>records_16</t>
-  </si>
-  <si>
-    <t>records_1</t>
   </si>
   <si>
     <t>records_32</t>
   </si>
   <si>
-    <t>records_80</t>
+    <t>records_64</t>
   </si>
   <si>
-    <t>records_64</t>
+    <t>records_80</t>
   </si>
   <si>
     <t>ebizzy_mmap_time</t>
@@ -3069,7 +3070,7 @@
       <c r="M29" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:M29"/>
+  <autoFilter ref="A2:M26"/>
   <mergeCells count="9">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A3:A26"/>
@@ -3099,8 +3100,8 @@
   </sheetPr>
   <dimension ref="1:53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4476,7 +4477,7 @@
   </sheetPr>
   <dimension ref="A1:AMI45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>

</xml_diff>